<commit_message>
Update homeless population by Gender.xlsx
</commit_message>
<xml_diff>
--- a/Data/homeless population by Gender.xlsx
+++ b/Data/homeless population by Gender.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1abe71445d0fcf/Documents/Data Scientist Program/Final Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1abe71445d0fcf/Documents/GitHub/Homelessness-Final-Group-Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{050C5D84-8DB2-436E-BA28-4CE0C320B291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F9294DE-0EC1-4AE8-A63F-554B94D1D02A}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{050C5D84-8DB2-436E-BA28-4CE0C320B291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37CC63BC-6221-482A-A83D-A51400B5E67A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3025A94-F23A-4E52-AD1B-070A21128C06}"/>
   </bookViews>
@@ -37,19 +37,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">        Gender non-conforming </t>
+    <t>Yeasrs</t>
   </si>
   <si>
-    <t xml:space="preserve">        Transgender people </t>
+    <t xml:space="preserve">Cisgender_women </t>
   </si>
   <si>
-    <t xml:space="preserve">        Cisgender men </t>
+    <t xml:space="preserve">Cisgender_men </t>
   </si>
   <si>
-    <t xml:space="preserve">        Cisgender women </t>
+    <t xml:space="preserve">Transgender_people </t>
   </si>
   <si>
-    <t xml:space="preserve">    By gender</t>
+    <t xml:space="preserve">Gender_non_conforming </t>
   </si>
 </sst>
 </file>
@@ -85,8 +85,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,123 +404,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A87E432-4E21-4441-9B59-29FD74F7151E}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>2015</v>
       </c>
-      <c r="C1">
+      <c r="B2" s="1">
+        <v>224344</v>
+      </c>
+      <c r="C2" s="1">
+        <v>339075</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1289</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2016</v>
       </c>
-      <c r="D1">
+      <c r="B3" s="1">
+        <v>217268</v>
+      </c>
+      <c r="C3" s="1">
+        <v>330890</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1770</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2017</v>
       </c>
-      <c r="E1">
+      <c r="B4" s="1">
+        <v>214975</v>
+      </c>
+      <c r="C4" s="1">
+        <v>333049</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2088</v>
+      </c>
+      <c r="E4" s="1">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2018</v>
       </c>
-      <c r="F1">
+      <c r="B5" s="1">
+        <v>216211</v>
+      </c>
+      <c r="C5" s="1">
+        <v>332925</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2521</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>2019</v>
       </c>
-      <c r="G1">
+      <c r="B6" s="1">
+        <v>219911</v>
+      </c>
+      <c r="C6" s="1">
+        <v>343187</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3255</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>2020</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>224344</v>
-      </c>
-      <c r="C2">
-        <v>217268</v>
-      </c>
-      <c r="D2">
-        <v>214975</v>
-      </c>
-      <c r="E2">
-        <v>216211</v>
-      </c>
-      <c r="F2">
-        <v>219911</v>
-      </c>
-      <c r="G2">
+      <c r="B7" s="1">
         <v>223578</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>339075</v>
-      </c>
-      <c r="C3">
-        <v>330890</v>
-      </c>
-      <c r="D3">
-        <v>333049</v>
-      </c>
-      <c r="E3">
-        <v>332925</v>
-      </c>
-      <c r="F3">
-        <v>343187</v>
-      </c>
-      <c r="G3">
+      <c r="C7" s="1">
         <v>352211</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1289</v>
-      </c>
-      <c r="C4">
-        <v>1770</v>
-      </c>
-      <c r="D4">
-        <v>2088</v>
-      </c>
-      <c r="E4">
-        <v>2521</v>
-      </c>
-      <c r="F4">
-        <v>3255</v>
-      </c>
-      <c r="G4">
+      <c r="D7" s="1">
         <v>3161</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>884</v>
-      </c>
-      <c r="E5">
-        <v>1173</v>
-      </c>
-      <c r="F5">
-        <v>1362</v>
-      </c>
-      <c r="G5">
+      <c r="E7" s="1">
         <v>1460</v>
       </c>
     </row>

</xml_diff>